<commit_message>
add some helper tables for moderator variables
</commit_message>
<xml_diff>
--- a/drafts/tables/TableXX_phosFract.xlsx
+++ b/drafts/tables/TableXX_phosFract.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/drafts/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733461E5-B64C-2048-9CE0-F5C7AA4113CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4F62BB-B03B-EB44-938F-207A255A5929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51760" yWindow="500" windowWidth="32460" windowHeight="17440" xr2:uid="{8C0274CA-637A-D549-8DE8-7F2B3B672490}"/>
+    <workbookView xWindow="36340" yWindow="500" windowWidth="32460" windowHeight="17440" xr2:uid="{8C0274CA-637A-D549-8DE8-7F2B3B672490}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,12 +99,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -128,16 +135,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -476,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A491FF-591D-5142-A76B-95AF05C56DB3}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,7 +537,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -553,71 +564,71 @@
       <c r="I2" s="1">
         <v>0.50600000000000001</v>
       </c>
-      <c r="J2" s="4" t="str">
+      <c r="J2" s="2" t="str">
         <f>CONCATENATE("[",H2,", ",I2,"]")</f>
         <v>[-1.928, 0.506]</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>1.022</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>0.34799999999999998</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>2.9409999999999998</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>0.34100000000000003</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="5">
         <v>1.7030000000000001</v>
       </c>
-      <c r="J3" s="4" t="str">
-        <f t="shared" ref="J3:J19" si="0">CONCATENATE("[",H3,", ",I3,"]")</f>
+      <c r="J3" s="6" t="str">
+        <f t="shared" ref="J3:J13" si="0">CONCATENATE("[",H3,", ",I3,"]")</f>
         <v>[0.341, 1.703]</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>0.56399999999999995</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>0.20499999999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>2.7480000000000002</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="5">
         <v>0.16200000000000001</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="5">
         <v>0.96599999999999997</v>
       </c>
-      <c r="J4" s="4" t="str">
+      <c r="J4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>[0.162, 0.966]</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
@@ -644,71 +655,71 @@
       <c r="I5" s="1">
         <v>0.24299999999999999</v>
       </c>
-      <c r="J5" s="4" t="str">
+      <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.026, 0.243]</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>0.40600000000000003</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>0.192</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>2.113</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="5">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="5">
         <v>0.78300000000000003</v>
       </c>
-      <c r="J6" s="4" t="str">
+      <c r="J6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>[0.029, 0.783]</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>0.34899999999999998</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="5">
         <v>0.16600000000000001</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <v>2.105</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="5">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="5">
         <v>2.4E-2</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="J7" s="4" t="str">
+      <c r="J7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>[0.024, 0.675]</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -735,13 +746,13 @@
       <c r="I8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J8" s="4" t="str">
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.141, 0.07]</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -764,13 +775,13 @@
       <c r="I9" s="1">
         <v>0.23200000000000001</v>
       </c>
-      <c r="J9" s="4" t="str">
+      <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.123, 0.232]</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -793,13 +804,13 @@
       <c r="I10" s="1">
         <v>0.57899999999999996</v>
       </c>
-      <c r="J10" s="4" t="str">
+      <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.166, 0.579]</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
@@ -826,13 +837,13 @@
       <c r="I11" s="1">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="J11" s="4" t="str">
+      <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.091, 0.092]</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -855,13 +866,13 @@
       <c r="I12" s="1">
         <v>0.20899999999999999</v>
       </c>
-      <c r="J12" s="4" t="str">
+      <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.068, 0.209]</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -884,7 +895,7 @@
       <c r="I13" s="1">
         <v>0.151</v>
       </c>
-      <c r="J13" s="4" t="str">
+      <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>[-0.058, 0.151]</v>
       </c>

</xml_diff>